<commit_message>
Documentation - Comment update
</commit_message>
<xml_diff>
--- a/SystemDevelopment/RelationalModel.xlsx
+++ b/SystemDevelopment/RelationalModel.xlsx
@@ -157,10 +157,10 @@
     <t>Country</t>
   </si>
   <si>
-    <t>ProductSupplierID</t>
-  </si>
-  <si>
     <t>zipCodeId</t>
+  </si>
+  <si>
+    <t>ProductSupplier</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G5" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
         <v>14</v>
       </c>
       <c r="O27" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P27" s="4" t="s">
         <v>16</v>

</xml_diff>